<commit_message>
test cases csv file
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebD\intern\reunion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E620B5-2FF2-4144-A70B-D9C346164334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02308F-7FF5-4CA6-BEBA-42A2ABA645A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4740AFC-9DB2-4828-A603-0153BAC73FE7}"/>
   </bookViews>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE0CC9D-B066-4AFD-AA56-8ED72E210351}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>

</xml_diff>